<commit_message>
Fixed tools, mrp, started fix for materials/parts sections
</commit_message>
<xml_diff>
--- a/templates/ETFSS MTA Template.xlsx
+++ b/templates/ETFSS MTA Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\OneDrive\Desktop\Dev Projects\MTA-Converter\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF7AB23-E18A-4FD2-8C8C-60F608DCE0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC09CC5-504F-4EC4-A7C1-44371643F0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{BF392F19-8E36-457E-8500-969E736579D9}"/>
+    <workbookView xWindow="57480" yWindow="7755" windowWidth="29040" windowHeight="15840" xr2:uid="{BF392F19-8E36-457E-8500-969E736579D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
   <si>
     <t>PLSN</t>
   </si>
@@ -163,16 +163,7 @@
 Custom 3/4" socket</t>
   </si>
   <si>
-    <t>THROUGH-WALL COUPLING 1/4" NPT I.D.
-1/4" NPT CLOSE NIPPLE
-1/4" FEMALE QUICK-DISCONNECT COUPLER
-1/4" FUEL NIPPLE (MALE Q/D)</t>
-  </si>
-  <si>
     <t>Side Flap, Vent Cover</t>
-  </si>
-  <si>
-    <t>STRIP, FOAM RUBBER, ADHESIVE-BACKED, NEOPRENE/EPDM/SBR. 1/8"THK, 1/2"WIDE, 4-5 FIRMNESS</t>
   </si>
   <si>
     <t>Cover, Exhaust Fan Terminal Block</t>
@@ -188,35 +179,43 @@
 SATS</t>
   </si>
   <si>
-    <t>RAG, WIPING</t>
-  </si>
-  <si>
-    <t>RM-CAULK-CLR
-RM-LOCTITE 242
-RIVET, BLIND, DOME HD. CLOSED END, ALUM/STEEL, 1/8"DIA x .126-.187 GRIP
-WASHER, RIVET BACK-UP, STAINLESS, 1/8ID,.375OD,.062THICK
-GLOVES, MEN'S AND WOMEN'S
-GOGGLES, INDUSTRIAL</t>
-  </si>
-  <si>
-    <t>TAPE, ANTISEIZING
-SEALING COMPOUND
-GLOVES, MEN'S AND WOMEN'S</t>
-  </si>
-  <si>
-    <t>GLOVES, MEN'S AND WOMEN'S</t>
-  </si>
-  <si>
-    <t>NUT, SELF-LOCKING, HEXAGON: NYLOCK 10-32, CRES</t>
-  </si>
-  <si>
     <t>GMTK
-RIVETER (SATS)
-STEDLADDER, 6-FT</t>
+Drill (SATS)</t>
   </si>
   <si>
     <t>GMTK
-DRILL (SATS)</t>
+Riveter (SATS)
+Stepladder, 6-FT</t>
+  </si>
+  <si>
+    <t>Gloves, Men's and Women's
+Sealing Compound
+Tape, Antiseizing</t>
+  </si>
+  <si>
+    <t>Caulking Compound
+Gloves, Men's and Women's</t>
+  </si>
+  <si>
+    <t>Rag, Wiping</t>
+  </si>
+  <si>
+    <t>Tape, Duct</t>
+  </si>
+  <si>
+    <t>Multimeter</t>
+  </si>
+  <si>
+    <t>Filter Element, Fluid</t>
+  </si>
+  <si>
+    <t>Nut, Self-Locking, Hexagon
+Rivet, Blind
+Washer, Lock</t>
+  </si>
+  <si>
+    <t>Nut, Self-Locking, Hexagon
+Washer, Lock</t>
   </si>
 </sst>
 </file>
@@ -498,99 +497,99 @@
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -913,7 +912,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -924,7 +923,7 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -944,345 +943,353 @@
     <col min="20" max="20" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="87" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4" t="s">
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="3" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3" t="s">
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="7" t="s">
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
+      <c r="A2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="P2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="R2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="S2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="14" t="s">
+      <c r="T2" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19" t="s">
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="11">
+        <v>1</v>
+      </c>
+      <c r="P3" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="17" t="s">
+      <c r="J4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="17">
+      <c r="N4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="2">
         <v>1</v>
       </c>
-      <c r="P3" s="21">
-        <v>0.2</v>
-      </c>
-      <c r="Q3" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T3" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="232.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="L4" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="M4" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="O4" s="25">
-        <v>1</v>
-      </c>
-      <c r="P4" s="27">
+      <c r="P4" s="19">
         <v>0.1</v>
       </c>
-      <c r="Q4" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="S4" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="T4" s="28" t="s">
+      <c r="Q4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="26" t="s">
+      <c r="G5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="25" t="s">
+      <c r="I5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="25" t="s">
+      <c r="N5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="O5" s="25">
+      <c r="O5" s="2">
         <v>1</v>
       </c>
-      <c r="P5" s="27">
+      <c r="P5" s="19">
         <v>0.1</v>
       </c>
-      <c r="Q5" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="R5" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="S5" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="T5" s="28" t="s">
+      <c r="Q5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5" s="20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="145" x14ac:dyDescent="0.35">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="25" t="s">
+      <c r="G6" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="L6" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="M6" s="25" t="s">
+      <c r="I6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="25" t="s">
+      <c r="N6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="O6" s="25">
+      <c r="O6" s="2">
         <v>2</v>
       </c>
-      <c r="P6" s="27">
+      <c r="P6" s="19">
         <v>0.1</v>
       </c>
-      <c r="Q6" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="R6" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="S6" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="T6" s="29" t="s">
+      <c r="Q6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T6" s="21" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="Q14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>